<commit_message>
Updated Duplicate Excel If Duplicate Movie Name detected, both orig and dupli will be saved in Duplicates.xlsx
</commit_message>
<xml_diff>
--- a/Duplicates.xlsx
+++ b/Duplicates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,39 +514,39 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>06</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>603.9 MB</t>
+          <t>590.18 MB</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The Flash</t>
+          <t>Baahubali Crown of Blood</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BluRay</t>
+          <t>1080p</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>x264</t>
+          <t>AVC</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Eng + Hin + Tam</t>
+          <t>Hin + Kan + Mal + Tam + Tel</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -562,7 +562,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>612.95 MB</t>
+          <t>603.9 MB</t>
         </is>
       </c>
     </row>
@@ -600,12 +600,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>05</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>641.95 MB</t>
+          <t>613.37 MB</t>
         </is>
       </c>
     </row>
@@ -643,12 +643,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>04</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>613.14 MB</t>
+          <t>612.95 MB</t>
         </is>
       </c>
     </row>
@@ -686,39 +686,39 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>01</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>612.69 MB</t>
+          <t>641.95 MB</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Baahubali Crown of Blood</t>
+          <t>The Flash</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1080p</t>
+          <t>BluRay</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>AVC</t>
+          <t>x264</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Hin + Kan + Mal + Tam + Tel</t>
+          <t>Eng + Hin + Tam</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -729,24 +729,24 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>601.64 MB</t>
+          <t>613.14 MB</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Deadpool &amp; Wolverine</t>
+          <t>The Flash</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -761,26 +761,30 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Eng + Hin + Tam + Tel</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>192Kbps &amp; DD+5.1</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+          <t>Eng + Hin + Tam</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1.66 GB</t>
+          <t>612.69 MB</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Meiyazhagan</t>
+          <t>Baahubali Crown of Blood</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -790,36 +794,40 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HQ HDRip</t>
+          <t>1080p</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>x264</t>
+          <t>AVC</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Tamil + Tamil - HQ HDRip - x264 - AAC - 700MB - ESub</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>AAC</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+          <t>Hin + Kan + Mal + Tam + Tel</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>739.14 MB</t>
+          <t>601.64 MB</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pushpa 2 The Rule</t>
+          <t>Deadpool &amp; Wolverine</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -829,36 +837,36 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1080p</t>
+          <t>4K</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>AVC</t>
+          <t>SDR</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Tamil + Tamil - 1080p HD AVC UNTOUCHED - x264 - AAC - 4.8GB</t>
+          <t>English</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>AAC</t>
+          <t>768Kbps &amp; AAC &amp; DD+5.1</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>4.84 GB</t>
+          <t>22.53 GB</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Miss You</t>
+          <t>Deadpool &amp; Wolverine</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -868,7 +876,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>720p</t>
+          <t>BluRay</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -878,26 +886,26 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>AAC + Tamil + Tamil - 720p HQ HDRip - x264 - [DD5.1(192Kbps)</t>
+          <t>Eng + Hin + Tam + Tel</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>AAC &amp; 192Kbps</t>
+          <t>192Kbps &amp; DD+5.1</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1.14 GB</t>
+          <t>1.66 GB</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Singham Again</t>
+          <t>Meiyazhagan</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -907,36 +915,36 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>720p</t>
+          <t>HQ HDRip</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>HEVC</t>
+          <t>x264</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>AAC + Tamil + Tamil - 720p HQ HDRip HEVC - x265 - [DD5.1(192Kbps)</t>
+          <t>Tamil + Tamil UNCUT - HQ HDRip - x264 - AAC - 700MB - ESub</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>AAC &amp; 192Kbps</t>
+          <t>AAC</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>984.75 MB</t>
+          <t>739.0 MB</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Barroz</t>
+          <t>Meiyazhagan</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -951,51 +959,51 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>HEVC</t>
+          <t>x264</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Tamil</t>
+          <t>Tamil + Tamil - HQ HDRip - x264 - AAC - 700MB - ESub</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>AAC &amp; 192Kbps &amp; DD+5.1</t>
+          <t>AAC</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1.1 GB</t>
+          <t>739.14 MB</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Game Changer</t>
+          <t>Pushpa 2 The Rule</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HQ HDRip</t>
+          <t>720p</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>HEVC</t>
+          <t>x264</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Tamil</t>
+          <t>Kannada + Kannada - 720p HDRip - x264 - AAC - 1.4GB - Original Audio</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1006,6 +1014,357 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
+        <is>
+          <t>1.42 GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Pushpa 2 The Rule</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1080p</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>AVC</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Tamil + Tamil - 1080p HD AVC UNTOUCHED - x264 - AAC - 4.8GB</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>AAC</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>4.84 GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Miss You</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>HQ HDRip</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>x265</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Tamil</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>AAC</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>909.73 MB</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Miss You</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>720p</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>x264</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>AAC + Tamil + Tamil - 720p HQ HDRip - x264 - [DD5.1(192Kbps)</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>AAC &amp; 192Kbps</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1.14 GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Singham Again</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>HQ HDRip</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>x264</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Hindi + Hindi - HQ HDRip - x264 - AAC - 800MB</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>AAC</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>837.42 MB</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Singham Again</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>720p</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>HEVC</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>AAC + Tamil + Tamil - 720p HQ HDRip HEVC - x265 - [DD5.1(192Kbps)</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>AAC &amp; 192Kbps</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>984.75 MB</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Barroz</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>720p</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>HEVC</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Tamil</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>AAC</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>972.66 MB</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Barroz</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>HQ HDRip</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>HEVC</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Tamil</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>AAC &amp; 192Kbps &amp; DD+5.1</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>1.1 GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Game Changer</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>720p</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>HEVC</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>AAC + Tamil + Tamil - 720p HQ HDRip HEVC - x265 - [DD5.1(192Kbps)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>AAC &amp; 192Kbps</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>1.26 GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Game Changer</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>HQ HDRip</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>HEVC</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Tamil</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>AAC</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
         <is>
           <t>957.45 MB</t>
         </is>

</xml_diff>